<commit_message>
Change excel sheet value
</commit_message>
<xml_diff>
--- a/seleniumDataSheet.xlsx
+++ b/seleniumDataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\Desktop\AtegrityAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D2B4953-36F2-4A4E-B348-AE82AC6B02E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B7FAC7-8B91-41BA-A4D0-4A99C1E4A707}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9AE26289-2D71-4407-A7DA-4D4CF7DCC553}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9AE26289-2D71-4407-A7DA-4D4CF7DCC553}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>Suresh</t>
   </si>
   <si>
-    <t>Mahesh</t>
+    <t>Vinesh</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>